<commit_message>
Added light guide to hardware BOM
</commit_message>
<xml_diff>
--- a/docs/assets/downloads/cae/pcb/gg-pcb-bom-v1.1.xlsx
+++ b/docs/assets/downloads/cae/pcb/gg-pcb-bom-v1.1.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="BOM_Main_Main_2025-11-19" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="BOM_Main_Main_2026-01-16" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="126">
   <si>
     <t>No.</t>
   </si>
@@ -187,6 +187,21 @@
     <t>8</t>
   </si>
   <si>
+    <t>1271.1000</t>
+  </si>
+  <si>
+    <t>LG1</t>
+  </si>
+  <si>
+    <t>MENTOR-1271.1000</t>
+  </si>
+  <si>
+    <t>MENTOR GmbH &amp; Co. Präzisions-Bauteile KG</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>560Ω</t>
   </si>
   <si>
@@ -205,7 +220,7 @@
     <t>C23204</t>
   </si>
   <si>
-    <t>9</t>
+    <t>10</t>
   </si>
   <si>
     <t>MST22D18G2 125</t>
@@ -223,7 +238,7 @@
     <t>C2906280</t>
   </si>
   <si>
-    <t>10</t>
+    <t>11</t>
   </si>
   <si>
     <t>MISO</t>
@@ -244,7 +259,7 @@
     <t>C238122</t>
   </si>
   <si>
-    <t>11</t>
+    <t>12</t>
   </si>
   <si>
     <t>MOSI</t>
@@ -253,7 +268,7 @@
     <t>TP4</t>
   </si>
   <si>
-    <t>12</t>
+    <t>13</t>
   </si>
   <si>
     <t>SCK</t>
@@ -262,7 +277,7 @@
     <t>TP5</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>CSN</t>
@@ -271,7 +286,7 @@
     <t>TP6</t>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
   <si>
     <t>GDO0</t>
@@ -280,7 +295,7 @@
     <t>TP7</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
   <si>
     <t>GPIO1</t>
@@ -289,7 +304,7 @@
     <t>TP8</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
   <si>
     <t>GPIO2</t>
@@ -298,7 +313,7 @@
     <t>TP9</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
   <si>
     <t>GPIO3</t>
@@ -307,7 +322,7 @@
     <t>TP10</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>GPIO4</t>
@@ -316,7 +331,7 @@
     <t>TP11</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>GND</t>
@@ -325,7 +340,7 @@
     <t>TP12</t>
   </si>
   <si>
-    <t>20</t>
+    <t>21</t>
   </si>
   <si>
     <t>E07-900M10S</t>
@@ -340,7 +355,7 @@
     <t>C9900007000</t>
   </si>
   <si>
-    <t>21</t>
+    <t>22</t>
   </si>
   <si>
     <t>L78M05ABDT-TR</t>
@@ -358,7 +373,7 @@
     <t>C58069</t>
   </si>
   <si>
-    <t>22</t>
+    <t>23</t>
   </si>
   <si>
     <t>AMS1117-3.3</t>
@@ -750,7 +765,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -1032,48 +1047,48 @@
         <v>60</v>
       </c>
       <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
         <v>58</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>61</v>
       </c>
-      <c r="H9" t="s">
-        <v>62</v>
-      </c>
       <c r="I9" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
         <v>64</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>65</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" t="s">
         <v>66</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>67</v>
       </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>68</v>
-      </c>
-      <c r="I10" t="s">
-        <v>69</v>
       </c>
       <c r="J10" t="s">
         <v>17</v>
@@ -1081,31 +1096,31 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
         <v>70</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>71</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>72</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" t="s">
         <v>73</v>
       </c>
-      <c r="F11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>74</v>
-      </c>
-      <c r="H11" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" t="s">
-        <v>76</v>
       </c>
       <c r="J11" t="s">
         <v>17</v>
@@ -1113,31 +1128,31 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" t="s">
         <v>77</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>78</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
         <v>79</v>
       </c>
-      <c r="E12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" t="s">
-        <v>74</v>
-      </c>
       <c r="H12" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I12" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="J12" t="s">
         <v>17</v>
@@ -1145,31 +1160,31 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" t="s">
         <v>80</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="I13" t="s">
         <v>81</v>
-      </c>
-      <c r="D13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" t="s">
-        <v>76</v>
       </c>
       <c r="J13" t="s">
         <v>17</v>
@@ -1177,31 +1192,31 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F14" t="s">
         <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="J14" t="s">
         <v>17</v>
@@ -1209,31 +1224,31 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F15" t="s">
         <v>36</v>
       </c>
       <c r="G15" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H15" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I15" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="J15" t="s">
         <v>17</v>
@@ -1241,31 +1256,31 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F16" t="s">
         <v>36</v>
       </c>
       <c r="G16" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H16" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I16" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="J16" t="s">
         <v>17</v>
@@ -1273,31 +1288,31 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
         <v>36</v>
       </c>
       <c r="G17" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H17" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I17" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="J17" t="s">
         <v>17</v>
@@ -1305,31 +1320,31 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F18" t="s">
         <v>36</v>
       </c>
       <c r="G18" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H18" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I18" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="J18" t="s">
         <v>17</v>
@@ -1337,31 +1352,31 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D19" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
         <v>36</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H19" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I19" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="J19" t="s">
         <v>17</v>
@@ -1369,31 +1384,31 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
         <v>36</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H20" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I20" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="J20" t="s">
         <v>17</v>
@@ -1401,31 +1416,31 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E21" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="F21" t="s">
         <v>36</v>
       </c>
       <c r="G21" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="H21" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="I21" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="J21" t="s">
         <v>17</v>
@@ -1454,10 +1469,10 @@
         <v>110</v>
       </c>
       <c r="H22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" t="s">
         <v>113</v>
-      </c>
-      <c r="I22" t="s">
-        <v>114</v>
       </c>
       <c r="J22" t="s">
         <v>17</v>
@@ -1465,38 +1480,70 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
         <v>115</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>116</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>117</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" t="s">
         <v>118</v>
       </c>
-      <c r="F23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" t="s">
-        <v>116</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>119</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>120</v>
       </c>
-      <c r="J23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H24" t="s">
+        <v>124</v>
+      </c>
+      <c r="I24" t="s">
+        <v>125</v>
+      </c>
+      <c r="J24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>